<commit_message>
Incorporates modeled vintages into power sector capacity tracking and introduces current and preceding modeled vintages
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/MV/Modeled Vintages.xlsx
+++ b/InputData/ctrl-settings/MV/Modeled Vintages.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\ctrl-settings\MV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C680B7A3-9ED9-4E29-8656-C5CE8EE045FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A24062D-AB69-4672-AD07-8F6E1FB50E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11175" activeTab="1" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
+    <workbookView xWindow="32205" yWindow="1185" windowWidth="24600" windowHeight="14205" activeTab="3" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="MV" sheetId="2" r:id="rId2"/>
+    <sheet name="MV-current" sheetId="3" r:id="rId3"/>
+    <sheet name="MV-preceding" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="264">
   <si>
     <t xml:space="preserve">Sources: </t>
   </si>
@@ -814,6 +816,18 @@
   </si>
   <si>
     <t>ModeledVintage2050</t>
+  </si>
+  <si>
+    <t>The MV-current tab defines the "current modeled vintage" subrange, and should</t>
+  </si>
+  <si>
+    <t>include all vintages after the initial year.</t>
+  </si>
+  <si>
+    <t>The MV-preceding tab defines the "preceding modeled vintage" subrange, and should</t>
+  </si>
+  <si>
+    <t>include all vintages except the final year.</t>
   </si>
 </sst>
 </file>
@@ -1180,20 +1194,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1D3264-BEAA-43D0-A5CC-06C5D3B72BE0}">
-  <dimension ref="A1:B160"/>
+  <dimension ref="A1:B166"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D15:D16"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1201,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1209,768 +1223,788 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A150" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1983,20 +2017,20 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CD6120-1A91-49A9-8DC0-F94251E02B6F}">
   <sheetPr>
-    <tabColor theme="4" tint="-0.499984740745262"/>
+    <tabColor rgb="FF0070C0"/>
   </sheetPr>
   <dimension ref="A1:B102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>158</v>
       </c>
@@ -2004,7 +2038,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>159</v>
       </c>
@@ -2012,7 +2046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -2020,7 +2054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -2028,7 +2062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>162</v>
       </c>
@@ -2036,7 +2070,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -2044,7 +2078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -2052,7 +2086,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -2060,7 +2094,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>166</v>
       </c>
@@ -2068,7 +2102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -2076,7 +2110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>168</v>
       </c>
@@ -2084,7 +2118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>169</v>
       </c>
@@ -2092,7 +2126,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>170</v>
       </c>
@@ -2100,7 +2134,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>171</v>
       </c>
@@ -2108,7 +2142,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>172</v>
       </c>
@@ -2116,7 +2150,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>173</v>
       </c>
@@ -2124,7 +2158,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>174</v>
       </c>
@@ -2132,7 +2166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>175</v>
       </c>
@@ -2140,7 +2174,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>176</v>
       </c>
@@ -2148,7 +2182,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>177</v>
       </c>
@@ -2156,7 +2190,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>178</v>
       </c>
@@ -2164,7 +2198,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>179</v>
       </c>
@@ -2172,7 +2206,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>180</v>
       </c>
@@ -2180,7 +2214,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>181</v>
       </c>
@@ -2188,7 +2222,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -2196,7 +2230,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>183</v>
       </c>
@@ -2204,7 +2238,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>184</v>
       </c>
@@ -2212,7 +2246,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>185</v>
       </c>
@@ -2220,7 +2254,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>186</v>
       </c>
@@ -2228,7 +2262,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>187</v>
       </c>
@@ -2236,7 +2270,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>188</v>
       </c>
@@ -2244,7 +2278,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>189</v>
       </c>
@@ -2252,7 +2286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>190</v>
       </c>
@@ -2260,7 +2294,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>191</v>
       </c>
@@ -2268,7 +2302,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>192</v>
       </c>
@@ -2276,7 +2310,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>193</v>
       </c>
@@ -2284,7 +2318,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>194</v>
       </c>
@@ -2292,7 +2326,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>195</v>
       </c>
@@ -2300,7 +2334,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>196</v>
       </c>
@@ -2308,7 +2342,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>197</v>
       </c>
@@ -2316,7 +2350,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>198</v>
       </c>
@@ -2324,7 +2358,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>199</v>
       </c>
@@ -2332,7 +2366,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>200</v>
       </c>
@@ -2340,7 +2374,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>201</v>
       </c>
@@ -2348,7 +2382,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>202</v>
       </c>
@@ -2356,7 +2390,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>203</v>
       </c>
@@ -2364,7 +2398,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>204</v>
       </c>
@@ -2372,7 +2406,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>205</v>
       </c>
@@ -2380,7 +2414,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>206</v>
       </c>
@@ -2388,7 +2422,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>207</v>
       </c>
@@ -2396,7 +2430,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>208</v>
       </c>
@@ -2404,7 +2438,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>209</v>
       </c>
@@ -2412,7 +2446,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>210</v>
       </c>
@@ -2420,7 +2454,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>211</v>
       </c>
@@ -2428,7 +2462,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>212</v>
       </c>
@@ -2436,7 +2470,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>213</v>
       </c>
@@ -2444,7 +2478,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>214</v>
       </c>
@@ -2452,7 +2486,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>215</v>
       </c>
@@ -2460,7 +2494,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>216</v>
       </c>
@@ -2468,7 +2502,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>217</v>
       </c>
@@ -2476,7 +2510,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>218</v>
       </c>
@@ -2484,7 +2518,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>219</v>
       </c>
@@ -2492,7 +2526,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>220</v>
       </c>
@@ -2500,7 +2534,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>221</v>
       </c>
@@ -2508,7 +2542,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>222</v>
       </c>
@@ -2516,7 +2550,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>223</v>
       </c>
@@ -2524,7 +2558,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>224</v>
       </c>
@@ -2532,7 +2566,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>225</v>
       </c>
@@ -2540,7 +2574,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>226</v>
       </c>
@@ -2548,7 +2582,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>227</v>
       </c>
@@ -2556,7 +2590,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>228</v>
       </c>
@@ -2564,7 +2598,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>229</v>
       </c>
@@ -2572,7 +2606,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>230</v>
       </c>
@@ -2580,7 +2614,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>231</v>
       </c>
@@ -2588,7 +2622,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>232</v>
       </c>
@@ -2596,7 +2630,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>233</v>
       </c>
@@ -2604,7 +2638,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>234</v>
       </c>
@@ -2612,7 +2646,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>235</v>
       </c>
@@ -2620,7 +2654,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>236</v>
       </c>
@@ -2628,7 +2662,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>237</v>
       </c>
@@ -2636,7 +2670,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>238</v>
       </c>
@@ -2644,7 +2678,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>239</v>
       </c>
@@ -2652,7 +2686,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>240</v>
       </c>
@@ -2660,7 +2694,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>241</v>
       </c>
@@ -2668,7 +2702,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>242</v>
       </c>
@@ -2676,7 +2710,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>243</v>
       </c>
@@ -2684,7 +2718,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>244</v>
       </c>
@@ -2692,7 +2726,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>245</v>
       </c>
@@ -2700,7 +2734,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>246</v>
       </c>
@@ -2708,7 +2742,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>247</v>
       </c>
@@ -2716,7 +2750,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>248</v>
       </c>
@@ -2724,7 +2758,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>249</v>
       </c>
@@ -2732,7 +2766,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>250</v>
       </c>
@@ -2740,7 +2774,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>251</v>
       </c>
@@ -2748,7 +2782,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>252</v>
       </c>
@@ -2756,7 +2790,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>253</v>
       </c>
@@ -2764,7 +2798,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>254</v>
       </c>
@@ -2772,7 +2806,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>255</v>
       </c>
@@ -2780,7 +2814,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>256</v>
       </c>
@@ -2788,7 +2822,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>257</v>
       </c>
@@ -2796,7 +2830,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>258</v>
       </c>
@@ -2804,7 +2838,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>259</v>
       </c>
@@ -2816,4 +2850,1054 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23289930-4E76-4095-89BB-5F236392D131}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:A101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8699E7D0-8410-4464-8069-D03CB76605DB}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:A101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>258</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adds new subranges for first vintage / first modeled vintage; modifies formula to read in vintage subscripts and subranges from input data
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/MV/Modeled Vintages.xlsx
+++ b/InputData/ctrl-settings/MV/Modeled Vintages.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\US\eps-us\InputData\ctrl-settings\MV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A24062D-AB69-4672-AD07-8F6E1FB50E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5EA5CF-754F-487E-818D-4C1FCEBCB68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32205" yWindow="1185" windowWidth="24600" windowHeight="14205" activeTab="3" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A7A9C5C-85FC-43FE-AB1B-A2C5DC00E496}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="MV" sheetId="2" r:id="rId2"/>
     <sheet name="MV-current" sheetId="3" r:id="rId3"/>
     <sheet name="MV-preceding" sheetId="4" r:id="rId4"/>
+    <sheet name="FMV" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="264">
   <si>
     <t xml:space="preserve">Sources: </t>
   </si>
@@ -1196,18 +1197,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A1D3264-BEAA-43D0-A5CC-06C5D3B72BE0}">
   <dimension ref="A1:B166"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1215,7 +1216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1223,787 +1224,787 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>157</v>
       </c>
@@ -2022,15 +2023,15 @@
   <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>158</v>
       </c>
@@ -2038,7 +2039,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>159</v>
       </c>
@@ -2046,7 +2047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -2054,7 +2055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>161</v>
       </c>
@@ -2062,7 +2063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>162</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -2078,7 +2079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -2086,7 +2087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -2094,7 +2095,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>166</v>
       </c>
@@ -2102,7 +2103,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -2110,7 +2111,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>168</v>
       </c>
@@ -2118,7 +2119,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>169</v>
       </c>
@@ -2126,7 +2127,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>170</v>
       </c>
@@ -2134,7 +2135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>171</v>
       </c>
@@ -2142,7 +2143,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>172</v>
       </c>
@@ -2150,7 +2151,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>173</v>
       </c>
@@ -2158,7 +2159,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>174</v>
       </c>
@@ -2166,7 +2167,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>175</v>
       </c>
@@ -2174,7 +2175,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>176</v>
       </c>
@@ -2182,7 +2183,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>177</v>
       </c>
@@ -2190,7 +2191,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>178</v>
       </c>
@@ -2198,7 +2199,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>179</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>180</v>
       </c>
@@ -2214,7 +2215,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>181</v>
       </c>
@@ -2222,7 +2223,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>182</v>
       </c>
@@ -2230,7 +2231,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>183</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>184</v>
       </c>
@@ -2246,7 +2247,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>185</v>
       </c>
@@ -2254,7 +2255,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>186</v>
       </c>
@@ -2262,7 +2263,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>187</v>
       </c>
@@ -2270,7 +2271,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>188</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>189</v>
       </c>
@@ -2286,7 +2287,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>190</v>
       </c>
@@ -2294,7 +2295,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>191</v>
       </c>
@@ -2302,7 +2303,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>192</v>
       </c>
@@ -2310,7 +2311,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>193</v>
       </c>
@@ -2318,7 +2319,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>194</v>
       </c>
@@ -2326,7 +2327,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>195</v>
       </c>
@@ -2334,7 +2335,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>196</v>
       </c>
@@ -2342,7 +2343,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>197</v>
       </c>
@@ -2350,7 +2351,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>198</v>
       </c>
@@ -2358,7 +2359,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>199</v>
       </c>
@@ -2366,7 +2367,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>200</v>
       </c>
@@ -2374,7 +2375,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>201</v>
       </c>
@@ -2382,7 +2383,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>202</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>203</v>
       </c>
@@ -2398,7 +2399,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>204</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>205</v>
       </c>
@@ -2414,7 +2415,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>206</v>
       </c>
@@ -2422,7 +2423,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>207</v>
       </c>
@@ -2430,7 +2431,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>208</v>
       </c>
@@ -2438,7 +2439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>209</v>
       </c>
@@ -2446,7 +2447,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>210</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>211</v>
       </c>
@@ -2462,7 +2463,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>212</v>
       </c>
@@ -2470,7 +2471,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>213</v>
       </c>
@@ -2478,7 +2479,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>214</v>
       </c>
@@ -2486,7 +2487,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>215</v>
       </c>
@@ -2494,7 +2495,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>216</v>
       </c>
@@ -2502,7 +2503,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>217</v>
       </c>
@@ -2510,7 +2511,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>218</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>219</v>
       </c>
@@ -2526,7 +2527,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>220</v>
       </c>
@@ -2534,7 +2535,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>221</v>
       </c>
@@ -2542,7 +2543,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>222</v>
       </c>
@@ -2550,7 +2551,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>223</v>
       </c>
@@ -2558,7 +2559,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>224</v>
       </c>
@@ -2566,7 +2567,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>225</v>
       </c>
@@ -2574,7 +2575,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>226</v>
       </c>
@@ -2582,7 +2583,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>227</v>
       </c>
@@ -2590,7 +2591,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>228</v>
       </c>
@@ -2598,7 +2599,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>229</v>
       </c>
@@ -2606,7 +2607,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>230</v>
       </c>
@@ -2614,7 +2615,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>231</v>
       </c>
@@ -2622,7 +2623,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>232</v>
       </c>
@@ -2630,7 +2631,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>233</v>
       </c>
@@ -2638,7 +2639,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>234</v>
       </c>
@@ -2646,7 +2647,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>235</v>
       </c>
@@ -2654,7 +2655,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>236</v>
       </c>
@@ -2662,7 +2663,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>237</v>
       </c>
@@ -2670,7 +2671,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>238</v>
       </c>
@@ -2678,7 +2679,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>239</v>
       </c>
@@ -2686,7 +2687,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>240</v>
       </c>
@@ -2694,7 +2695,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>241</v>
       </c>
@@ -2702,7 +2703,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>242</v>
       </c>
@@ -2710,7 +2711,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>243</v>
       </c>
@@ -2718,7 +2719,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>244</v>
       </c>
@@ -2726,7 +2727,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>245</v>
       </c>
@@ -2734,7 +2735,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>246</v>
       </c>
@@ -2742,7 +2743,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>247</v>
       </c>
@@ -2750,7 +2751,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>248</v>
       </c>
@@ -2758,7 +2759,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>249</v>
       </c>
@@ -2766,7 +2767,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>250</v>
       </c>
@@ -2774,7 +2775,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>251</v>
       </c>
@@ -2782,7 +2783,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>252</v>
       </c>
@@ -2790,7 +2791,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>253</v>
       </c>
@@ -2798,7 +2799,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>254</v>
       </c>
@@ -2806,7 +2807,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>255</v>
       </c>
@@ -2814,7 +2815,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>256</v>
       </c>
@@ -2822,7 +2823,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>257</v>
       </c>
@@ -2830,7 +2831,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>258</v>
       </c>
@@ -2838,7 +2839,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>259</v>
       </c>
@@ -2861,512 +2862,512 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>259</v>
       </c>
@@ -3383,518 +3384,547 @@
   </sheetPr>
   <dimension ref="A1:A101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>258</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{959C1722-33B8-474E-9713-0BE58AA8F260}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>MV!A2</f>
+        <v>ModeledVintage1950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>